<commit_message>
Update conference data and improve date format handling
- Enhanced parse_date() to handle timestamp format (YYYY-MM-DD HH:MM:SS)
- Strip time component from DDL display for cleaner presentation
- Updated conference listings with new entries and filtered past deadlines
- Updated conferences.xlsx data file

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/files/conferences.xlsx
+++ b/files/conferences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hulaizh/finance-conferences/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A6F44B-FC1C-D04C-879C-D7237F5B8018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AD6A07-1D81-7544-99AB-2059301BACEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="228">
   <si>
     <t>name</t>
   </si>
@@ -52,7 +52,7 @@
     <t>2025-12-11 to 2025-12-12</t>
   </si>
   <si>
-    <t>2025-08-27</t>
+    <t>2025-08-27 00:00:00</t>
   </si>
   <si>
     <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17258</t>
@@ -67,6 +67,9 @@
     <t>2025-08-30</t>
   </si>
   <si>
+    <t>2025-08-30 00:00:00</t>
+  </si>
+  <si>
     <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17311</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
     <t>2025-08-31</t>
   </si>
   <si>
+    <t>2025-08-31 00:00:00</t>
+  </si>
+  <si>
     <t>https://sfs.org/wp-content/uploads/2025/07/Call_for_papers_CUHK-RAPS-RCFS-Conference_2025.pdf</t>
   </si>
   <si>
@@ -139,6 +145,9 @@
     <t>2025-09-01</t>
   </si>
   <si>
+    <t>2025-09-01 00:00:00</t>
+  </si>
+  <si>
     <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17593</t>
   </si>
   <si>
@@ -160,6 +169,9 @@
     <t>2025-09-05</t>
   </si>
   <si>
+    <t>2025-09-05 00:00:00</t>
+  </si>
+  <si>
     <t>https://mfa.memberclicks.net/2026-conference-paper-submission</t>
   </si>
   <si>
@@ -172,42 +184,45 @@
     <t>2025-12-13 to 2025-12-14</t>
   </si>
   <si>
+    <t>2025-09-15 00:00:00</t>
+  </si>
+  <si>
+    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17558</t>
+  </si>
+  <si>
+    <t>9th Commodity Markets Winter Workshop</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Brand, Austria</t>
+  </si>
+  <si>
+    <t>2026-02-03 to 2026-02-05</t>
+  </si>
+  <si>
+    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17478</t>
+  </si>
+  <si>
+    <t>The 19th International Behavioural Finance Conference</t>
+  </si>
+  <si>
+    <t>2025-10-30 to 2025-10-31</t>
+  </si>
+  <si>
+    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17468</t>
+  </si>
+  <si>
+    <t>Sustainable Finance Research Forum Paris 2025</t>
+  </si>
+  <si>
+    <t>Paris, France</t>
+  </si>
+  <si>
     <t>2025-09-15</t>
   </si>
   <si>
-    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17558</t>
-  </si>
-  <si>
-    <t>9th Commodity Markets Winter Workshop</t>
-  </si>
-  <si>
-    <t>Europe</t>
-  </si>
-  <si>
-    <t>Brand, Austria</t>
-  </si>
-  <si>
-    <t>2026-02-03 to 2026-02-05</t>
-  </si>
-  <si>
-    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17478</t>
-  </si>
-  <si>
-    <t>The 19th International Behavioural Finance Conference</t>
-  </si>
-  <si>
-    <t>2025-10-30 to 2025-10-31</t>
-  </si>
-  <si>
-    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17468</t>
-  </si>
-  <si>
-    <t>Sustainable Finance Research Forum Paris 2025</t>
-  </si>
-  <si>
-    <t>Paris, France</t>
-  </si>
-  <si>
     <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17391</t>
   </si>
   <si>
@@ -226,6 +241,9 @@
     <t>2025-09-28</t>
   </si>
   <si>
+    <t>2025-09-28 00:00:00</t>
+  </si>
+  <si>
     <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17435</t>
   </si>
   <si>
@@ -238,18 +256,21 @@
     <t>2026-03-25 to 2026-03-28</t>
   </si>
   <si>
+    <t>2025-09-30 00:00:00</t>
+  </si>
+  <si>
+    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17579</t>
+  </si>
+  <si>
+    <t>The 2026 NYSE Market Microstructure Conference</t>
+  </si>
+  <si>
+    <t>New York Stock Exchange, 11 Wall St, New York, NY 10005, USA</t>
+  </si>
+  <si>
     <t>2025-09-30</t>
   </si>
   <si>
-    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17579</t>
-  </si>
-  <si>
-    <t>The 2026 NYSE Market Microstructure Conference</t>
-  </si>
-  <si>
-    <t>New York Stock Exchange, 11 Wall St, New York, NY 10005, USA</t>
-  </si>
-  <si>
     <t>https://www.nyse.com/events-2026-nyse-market-microstructure-conference</t>
   </si>
   <si>
@@ -262,7 +283,7 @@
     <t>2026-03-05 to 2026-03-07</t>
   </si>
   <si>
-    <t>2025-10-01</t>
+    <t>2025-10-01 00:00:00</t>
   </si>
   <si>
     <t>http://editorialexpress.com/conference/FDU2026</t>
@@ -277,7 +298,7 @@
     <t>2026-03-25 to 2026-03-27</t>
   </si>
   <si>
-    <t>2025-10-15</t>
+    <t>2025-10-15 00:00:00</t>
   </si>
   <si>
     <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17484</t>
@@ -298,7 +319,10 @@
     <t>Saas-Fee, 3906 Saas-Fee, Switzerland</t>
   </si>
   <si>
-    <t>2025-10-19</t>
+    <t>March 15 - 18, 2026</t>
+  </si>
+  <si>
+    <t>2025-10-19 00:00:00</t>
   </si>
   <si>
     <t>https://www.conftool.com/ewfs2026/</t>
@@ -313,7 +337,7 @@
     <t>2026-04-21 to 2026-04-23</t>
   </si>
   <si>
-    <t>2025-10-22</t>
+    <t>2025-10-22 00:00:00</t>
   </si>
   <si>
     <t>https://www.ssrn.com/</t>
@@ -325,7 +349,7 @@
     <t>SIX ConventionPoint, Pfingstweidstrasse 110, 8005 Zürich, Switz</t>
   </si>
   <si>
-    <t>2025-10-31</t>
+    <t>2025-10-31 00:00:00</t>
   </si>
   <si>
     <t>https://www.df.uzh.ch/en/news-events/events/2026/2026-SGF-conference.html</t>
@@ -340,7 +364,7 @@
     <t>2026-03-04 to 2026-03-07</t>
   </si>
   <si>
-    <t>2025-11-01</t>
+    <t>2025-11-01 00:00:00</t>
   </si>
   <si>
     <t>https://www.brettonwoodsskiconference.com/</t>
@@ -349,7 +373,13 @@
     <t>WEFIDEV RFS-CEPR Conference</t>
   </si>
   <si>
-    <t>2025-11-16</t>
+    <t>Kelloge, 2211 N Campus Dr, Evanston, IL 60208, US</t>
+  </si>
+  <si>
+    <t>April 18th and 19th, 2026</t>
+  </si>
+  <si>
+    <t>2025-11-16 00:00:00</t>
   </si>
   <si>
     <t>https://lnkd.in/eF6p4dHZ</t>
@@ -358,7 +388,10 @@
     <t>The Geoeconomics of Financial Markets Conference</t>
   </si>
   <si>
-    <t>2025-12-01</t>
+    <t>Stanford Graduate School of Business</t>
+  </si>
+  <si>
+    <t>2025-12-01 00:00:00</t>
   </si>
   <si>
     <t>https://lnkd.in/e_bAxEgg</t>
@@ -373,20 +406,314 @@
     <t>2026-04-15 to 2026-04-17</t>
   </si>
   <si>
-    <t>2025-12-15</t>
+    <t>2025-12-15 00:00:00</t>
   </si>
   <si>
     <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17456</t>
   </si>
   <si>
-    <t>Kelloge, 2211 N Campus Dr, Evanston, IL 60208, US</t>
+    <t>ASU Sonoran Winter Finance Conference 2026</t>
+  </si>
+  <si>
+    <t>Omni Montelucia, Scottsdale, Arizona</t>
+  </si>
+  <si>
+    <t>26 Feb 2026 - 28 Feb 2026</t>
+  </si>
+  <si>
+    <t>https://finance-conference.wpcarey.asu.edu/</t>
+  </si>
+  <si>
+    <t>The Friends of Women in Finance 4th Symposium in Greater New York (FWFS-GNY)</t>
+  </si>
+  <si>
+    <t>Hofstra University, Hempstead, New York, USA</t>
+  </si>
+  <si>
+    <t>https://forms.gle/CrtogGZmf14X9z5o9</t>
+  </si>
+  <si>
+    <t>Alternative Investments Conference &amp; IPC Current Issues in Alternatives Research Symposium</t>
+  </si>
+  <si>
+    <t>Chapel Hill, NC</t>
+  </si>
+  <si>
+    <t>26 Mar 2026 - 27 Mar 2026</t>
+  </si>
+  <si>
+    <t>https://uncipc.org/index.php/research/call-for-papers/</t>
+  </si>
+  <si>
+    <t>RBF Global Finance Forum 2026</t>
+  </si>
+  <si>
+    <t>Al-Hasa, King Faisal University, Saudi Arabia</t>
+  </si>
+  <si>
+    <t>31 Jan 2026 - 01 Feb 2026</t>
+  </si>
+  <si>
+    <t>https://cmt3.research.microsoft.com/User/Login?ReturnUrl=%2FRBFW2026%2F</t>
+  </si>
+  <si>
+    <t>Second Winter Finance Summit in Asia</t>
+  </si>
+  <si>
+    <t>Appi Resort, Japan</t>
+  </si>
+  <si>
+    <t>16 Feb 2026 - 19 Feb 2026</t>
+  </si>
+  <si>
+    <t>https://forms.gle/KTfHaGU1AucTHhF69</t>
+  </si>
+  <si>
+    <t>13th Annual Conference on Financial Market Regulation (CFMR 2026)</t>
+  </si>
+  <si>
+    <t>SEC Headquarters, Washington, DC</t>
+  </si>
+  <si>
+    <t>07 May 2026 - 08 May 2026</t>
+  </si>
+  <si>
+    <t>www.conftool.org/cfmr2026</t>
+  </si>
+  <si>
+    <t>RCFS Winter Conference</t>
+  </si>
+  <si>
+    <t>Royal Sonesta, San Juan, Puerto Rico</t>
+  </si>
+  <si>
+    <t>13 Feb 2026 - 15 Feb 2026</t>
+  </si>
+  <si>
+    <t>https://sfs.org/rcfs-winter-conference-2026/</t>
+  </si>
+  <si>
+    <t>2026 UBC Winter Finance Conference</t>
+  </si>
+  <si>
+    <t>Whistler, BC, Canada</t>
+  </si>
+  <si>
+    <t>27 Feb 2026 - 01 Mar 2026</t>
+  </si>
+  <si>
+    <t>https://webforms.sauder.ubc.ca/finance-conference-papers</t>
+  </si>
+  <si>
+    <t>Institute for Quantitative Investment Research Joint UK-Europe Spring Residential Seminar 2026</t>
+  </si>
+  <si>
+    <t>University Arms Hotel, Cambridge, U.K.</t>
+  </si>
+  <si>
+    <t>22 Mar 2026 - 24 Mar 2026</t>
+  </si>
+  <si>
+    <t>https://forms.gle/168fccQHU157Sfbq7</t>
+  </si>
+  <si>
+    <t>2026 Georgia Tech-Atlanta Fed Household Finance Conference</t>
+  </si>
+  <si>
+    <t>Atlanta, Georgia</t>
+  </si>
+  <si>
+    <t>https://gatech.co1.qualtrics.com/jfe/form/SV_894fk7MELugykhE</t>
+  </si>
+  <si>
+    <t>Baruch-JFQA Climate Finance and Sustainability Conference</t>
+  </si>
+  <si>
+    <t>Baruch College, City University of New York</t>
+  </si>
+  <si>
+    <t>12 Mar 2026 - 13 Mar 2026</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/view/baruch-jfqa-climate-finance-an/home</t>
+  </si>
+  <si>
+    <t>12th International Conference on Sovereign Bond Markets</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>02 Jun 2026 - 03 Jun 2026</t>
+  </si>
+  <si>
+    <t>https://www.greta.it/index.php/en/sbm-2026</t>
+  </si>
+  <si>
+    <t>Energy Finance and Climate Transition Risk Conference</t>
+  </si>
+  <si>
+    <t>University of North Carolina</t>
+  </si>
+  <si>
+    <t>09 Apr 2026 - 10 Apr 2026</t>
+  </si>
+  <si>
+    <t>https://www.kenan-flagler.unc.edu/energy-finance-and-climate-transition-risk/</t>
+  </si>
+  <si>
+    <t>WORLD FINANCE CONFERENCE -IRELAND</t>
+  </si>
+  <si>
+    <t>University of Limerick, Ireland</t>
+  </si>
+  <si>
+    <t>26 Jul 2026 - 29 Jul 2026</t>
+  </si>
+  <si>
+    <t>https://www.world-finance-conference.com/conference.php?id=32</t>
+  </si>
+  <si>
+    <t>Central Bank Payments Conference</t>
+  </si>
+  <si>
+    <t>Istanbul, Türkiye</t>
+  </si>
+  <si>
+    <t>23 Mar 2026 - 25 Mar 2026</t>
+  </si>
+  <si>
+    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17802</t>
+  </si>
+  <si>
+    <t>7th Analyst Research Conference</t>
+  </si>
+  <si>
+    <t>University of Notre Dame; Notre Dame, IN, USA</t>
+  </si>
+  <si>
+    <t>16 Apr 2026 - 17 Apr 2026</t>
+  </si>
+  <si>
+    <t>https://nd.qualtrics.com/jfe/form/SV_b3YyHuu30HcpFnU</t>
+  </si>
+  <si>
+    <t>Villanova School of Business MARC</t>
+  </si>
+  <si>
+    <t>Villanova, PA</t>
+  </si>
+  <si>
+    <t>https://vsbevents.villanova.edu/855553</t>
+  </si>
+  <si>
+    <t>Joint World Bank - Financial Analysts Journal Conference on “Public Asset Management: Best Practices and Innovations for the Future”</t>
+  </si>
+  <si>
+    <t>World Bank Headquarters, Washington DC, USA</t>
+  </si>
+  <si>
+    <t>16 Mar 2026 - 17 Mar 2026</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/journals/ufaj</t>
+  </si>
+  <si>
+    <t>Seventh Edinburgh Corporate Finance Conference</t>
+  </si>
+  <si>
+    <t>Edinburgh, Scotland</t>
+  </si>
+  <si>
+    <t>24 May 2026 - 25 May 2026</t>
+  </si>
+  <si>
+    <t>ecfc.business-school.ed.ac.uk</t>
+  </si>
+  <si>
+    <t>Federal Reserve Bank of Philadelphia Mortgage Market Research Conference</t>
+  </si>
+  <si>
+    <t>Federal Reserve Bank of Philadelphia</t>
+  </si>
+  <si>
+    <t>14 May 2026 - 15 May 2026</t>
+  </si>
+  <si>
+    <t>https://cvent.me/kY0mYR</t>
+  </si>
+  <si>
+    <t>2026 ITAM Finance Conference</t>
+  </si>
+  <si>
+    <t>ITAM Campus, Mexico City</t>
+  </si>
+  <si>
+    <t>20 Feb 2026 - 21 Feb 2026</t>
+  </si>
+  <si>
+    <t>https://gonzo.itam.mx/finance/Home/form0</t>
+  </si>
+  <si>
+    <t>19th Annual Corporate Governance Academic Conference at Drexel University</t>
+  </si>
+  <si>
+    <t>Philadelphia, PA</t>
+  </si>
+  <si>
+    <t>https://www.lebow.drexel.edu/event/2025/07/17/raj-kamla-gupta-governance-institute-drexel-university-2026-academic-conference</t>
+  </si>
+  <si>
+    <t>Ninth Duke-UNC Asset Pricing Conference</t>
+  </si>
+  <si>
+    <t>Duke University - Durham, North Carolina</t>
+  </si>
+  <si>
+    <t>27 Mar 2026 - 28 Mar 2026</t>
+  </si>
+  <si>
+    <t>https://conferences.fuqua.duke.edu/assetpricing/</t>
+  </si>
+  <si>
+    <t>2026 Loyola Wealth Management Conference</t>
+  </si>
+  <si>
+    <t>Loyola University Maryland</t>
+  </si>
+  <si>
+    <t>https://www.loyola.edu/sellinger-business/academics/departments/finance/events.html</t>
+  </si>
+  <si>
+    <t>Columbia/BPI Annual Bank Regulation Research Conference</t>
+  </si>
+  <si>
+    <t>Columbia University, New York City</t>
+  </si>
+  <si>
+    <t>https://www.ssrn.com/index.cfm/en/janda/announcement/?id=17719</t>
+  </si>
+  <si>
+    <t>5th Edition Spring Finance Workshop</t>
+  </si>
+  <si>
+    <t>Ischgl, Austria</t>
+  </si>
+  <si>
+    <t>19 Apr 2026 - 21 Apr 2026</t>
+  </si>
+  <si>
+    <t>www.springfinanceworkshop.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,9 +722,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="30"/>
+      <color rgb="FF222222"/>
+      <name val="NexusSerifWebPro"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF232323"/>
+      <name val="NexusSansWebPro"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF232323"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4C4C4C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -420,14 +786,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,43 +1108,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E19" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="53.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="4" customWidth="1"/>
     <col min="6" max="6" width="69.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -779,14 +1157,14 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -799,529 +1177,1057 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
       <c r="F10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" t="s">
-        <v>50</v>
-      </c>
       <c r="F13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>50</v>
+        <v>66</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
+        <v>66</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
+        <v>72</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" t="s">
-        <v>72</v>
+        <v>77</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" t="s">
-        <v>72</v>
+        <v>82</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" t="s">
-        <v>80</v>
+        <v>86</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" t="s">
-        <v>85</v>
+        <v>91</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" t="s">
-        <v>85</v>
+        <v>95</v>
+      </c>
+      <c r="D22" s="6">
+        <v>46060</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="F22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" t="s">
-        <v>92</v>
+        <v>98</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" t="s">
-        <v>97</v>
+        <v>104</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="F24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" t="s">
-        <v>101</v>
+        <v>108</v>
+      </c>
+      <c r="D25" s="8">
+        <v>46108</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="F25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" t="s">
-        <v>106</v>
+        <v>113</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="F26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D27" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" t="s">
-        <v>109</v>
-      </c>
       <c r="F27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" t="s">
-        <v>112</v>
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="5">
+        <v>46157</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D29" t="s">
-        <v>116</v>
-      </c>
-      <c r="E29" t="s">
-        <v>117</v>
+        <v>127</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="F29" t="s">
-        <v>118</v>
-      </c>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="4">
+        <v>45980</v>
+      </c>
+      <c r="F30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="6">
+        <v>46003</v>
+      </c>
+      <c r="E31" s="4">
+        <v>45964</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="4">
+        <v>45979</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="4">
+        <v>45991</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="4">
+        <v>45949</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="4">
+        <v>45979</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" s="4">
+        <v>45979</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E37" s="4">
+        <v>45980</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="4">
+        <v>45962</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="4">
+        <v>45979</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E40" s="4">
+        <v>45979</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" s="4">
+        <v>46006</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E42" s="4">
+        <v>45979</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E43" s="4">
+        <v>46082</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E44" s="4">
+        <v>45996</v>
+      </c>
+      <c r="F44" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E45" s="4">
+        <v>45992</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D46" s="6">
+        <v>46101</v>
+      </c>
+      <c r="E46" s="4">
+        <v>46006</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E47" s="4">
+        <v>45996</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E48" s="4">
+        <v>45963</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E49" s="4">
+        <v>46042</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E50" s="4">
+        <v>45949</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D51" s="6">
+        <v>46129</v>
+      </c>
+      <c r="E51" s="4">
+        <v>46013</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E52" s="4">
+        <v>45979</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D53" s="6">
+        <v>46108</v>
+      </c>
+      <c r="E53" s="4">
+        <v>46013</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D54" s="6">
+        <v>46073</v>
+      </c>
+      <c r="E54" s="4">
+        <v>45976</v>
+      </c>
+      <c r="F54" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="E55" s="4">
+        <v>45970</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="38" customHeight="1">
+      <c r="A56" s="2"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>